<commit_message>
EPBDS-11915 inherit index field from super datatype if it's present
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/EPBDS-9764/EPBDS-9764/EPBDS-9764_TransientFields.xlsx
+++ b/ITEST/itest.WebService/openl-repository/EPBDS-9764/EPBDS-9764/EPBDS-9764_TransientFields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9737_TransientFields\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets\ITEST\itest.WebService\openl-repository\EPBDS-9764\EPBDS-9764\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB350876-0255-4060-9CD3-77AD8BCC6505}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF62E6C-30B6-4275-A093-1A6DF50920AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4313" yWindow="833" windowWidth="19252" windowHeight="13470" tabRatio="878" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="44" r:id="rId1"/>
@@ -334,9 +334,6 @@
     <t>_res_.$Step16</t>
   </si>
   <si>
-    <t>= MyType1Data["value5"].field1</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult myMethod2(MyType1 myType1, MyType2 myType2, MyType3 myType3, MyType4 myType4)</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>Test myMethod6 myMethod6Test</t>
+  </si>
+  <si>
+    <t>= MyType1Data["2"].field1</t>
   </si>
 </sst>
 </file>
@@ -905,15 +905,15 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.78515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.35546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:12" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="8" t="s">
         <v>86</v>
@@ -930,7 +930,7 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -979,7 +979,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -988,7 +988,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -996,7 +996,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1004,7 +1004,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
         <v>80</v>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -1036,7 +1036,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,15 +1052,15 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="8" t="s">
         <v>79</v>
       </c>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1098,25 +1098,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>63</v>
       </c>
@@ -1132,28 +1132,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.5">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.5">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.5">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C36" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="6"/>
       <c r="G36" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.5">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C37" s="6" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6" t="s">
@@ -1171,10 +1171,10 @@
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>4</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6" t="s">
@@ -1192,7 +1192,7 @@
         <v>78</v>
       </c>
       <c r="I38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1215,13 +1215,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8B3E7E-BAAD-4041-AF0A-0225C6DEE82D}">
   <dimension ref="B4:M97"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>65</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1336,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1349,7 +1349,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1388,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1401,7 +1401,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1414,7 +1414,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>67</v>
       </c>
@@ -1427,15 +1427,15 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -1443,9 +1443,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1459,7 +1459,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1477,12 +1477,12 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1495,12 +1495,12 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1513,12 +1513,12 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1531,12 +1531,12 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1549,12 +1549,12 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1567,12 +1567,12 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1585,12 +1585,12 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1603,12 +1603,12 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1621,12 +1621,12 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1639,12 +1639,12 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1657,12 +1657,12 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1675,12 +1675,12 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1693,12 +1693,12 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1711,12 +1711,12 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1729,7 +1729,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1"/>
@@ -1743,7 +1743,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="3"/>
       <c r="D45" s="1"/>
@@ -1757,9 +1757,9 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1767,7 +1767,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>9</v>
       </c>
@@ -1779,151 +1779,151 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="3"/>
       <c r="D64" s="1"/>
@@ -1931,7 +1931,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="3"/>
       <c r="D65" s="1"/>
@@ -1939,9 +1939,9 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -1950,7 +1950,7 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="6" t="s">
         <v>9</v>
       </c>
@@ -1963,12 +1963,12 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B70" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
@@ -1976,12 +1976,12 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -1989,12 +1989,12 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
@@ -2002,12 +2002,12 @@
       <c r="G72" s="6"/>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
@@ -2015,12 +2015,12 @@
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B74" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -2028,12 +2028,12 @@
       <c r="G74" s="6"/>
       <c r="H74" s="6"/>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B75" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
@@ -2041,7 +2041,7 @@
       <c r="G75" s="6"/>
       <c r="H75" s="6"/>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" s="6"/>
       <c r="C76" s="3"/>
       <c r="D76" s="6"/>
@@ -2050,7 +2050,7 @@
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B77" s="6"/>
       <c r="C77" s="3"/>
       <c r="D77" s="6"/>
@@ -2059,7 +2059,7 @@
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B78" s="6"/>
       <c r="C78" s="3"/>
       <c r="D78" s="6"/>
@@ -2068,7 +2068,7 @@
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B79" s="6"/>
       <c r="C79" s="3"/>
       <c r="D79" s="6"/>
@@ -2077,9 +2077,9 @@
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B80" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -2088,7 +2088,7 @@
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B81" s="6" t="s">
         <v>9</v>
       </c>
@@ -2101,57 +2101,57 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B82" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B83" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B84" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B85" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B86" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.5">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B87" s="6"/>
       <c r="C87" s="3"/>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B91" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C91" s="6"/>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B92" s="6" t="s">
         <v>9</v>
       </c>
@@ -2159,44 +2159,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.5">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B93" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B94" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B95" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B96" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2213,9 +2213,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2223,7 +2223,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2231,7 +2231,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="7" t="s">
         <v>54</v>
@@ -2241,7 +2241,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>87</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>87</v>
@@ -2276,7 +2276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>1</v>
@@ -2294,7 +2294,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>2</v>
@@ -2312,7 +2312,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2320,7 +2320,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2328,7 +2328,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2336,7 +2336,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2344,7 +2344,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2352,7 +2352,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>55</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>56</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>50</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>1</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>57</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>1</v>
       </c>
@@ -2488,7 +2488,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>88</v>
       </c>
@@ -2514,18 +2514,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B787BA0A-80DD-4382-9E0D-AB692BB40CDA}">
   <dimension ref="A5:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I63" sqref="I62:I63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="9.140625" style="1" collapsed="1"/>
     <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
     <col min="14" max="15" width="9.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2538,7 +2538,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2551,7 +2551,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>60</v>
@@ -2580,7 +2580,7 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>35</v>
@@ -2648,7 +2648,7 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>57</v>
@@ -2683,7 +2683,7 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>77</v>
@@ -2751,7 +2751,7 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>1</v>
       </c>
@@ -2818,9 +2818,9 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2842,7 +2842,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
@@ -2901,7 +2901,7 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
@@ -2931,7 +2931,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>1</v>
       </c>
@@ -3049,9 +3049,9 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -3068,7 +3068,7 @@
       <c r="P29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>57</v>
       </c>
@@ -3139,7 +3139,7 @@
       <c r="P31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>77</v>
       </c>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>1</v>
       </c>
@@ -3198,46 +3198,46 @@
         <v>50</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R33" s="1"/>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -3255,7 +3255,7 @@
       <c r="P42" s="6"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
         <v>38</v>
       </c>
@@ -3281,7 +3281,7 @@
       <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
@@ -3307,7 +3307,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B45" s="6" t="s">
         <v>50</v>
       </c>
@@ -3333,7 +3333,7 @@
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -3351,14 +3351,14 @@
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
         <v>38</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="6" t="s">
         <v>11</v>
       </c>
@@ -3386,28 +3386,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="D54" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.5">
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="6" t="s">
         <v>38</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="6" t="s">
         <v>11</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="6" t="s">
         <v>50</v>
       </c>

</xml_diff>